<commit_message>
[fixed_asset template] missing subtotal
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
@@ -5,98 +5,103 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="88" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
-  <si>
-    <t>Depreciation Schedule</t>
-  </si>
-  <si>
-    <t>{{company_name}}</t>
-  </si>
-  <si>
-    <t>From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Purchase Price</t>
-  </si>
-  <si>
-    <t>Purchase Date</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Book Value
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">Depreciation Schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{company_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book Value
 {{fmt_date date_from}}</t>
   </si>
   <si>
-    <t>Accum Dep</t>
-  </si>
-  <si>
-    <t>Book Value {{fmt_date date_to}}</t>
-  </si>
-  <si>
-    <t>{{#each groups}}</t>
-  </si>
-  <si>
-    <t>{{type_name}}</t>
-  </si>
-  <si>
-    <t>{{#each lines}}</t>
-  </si>
-  <si>
-    <t>{{asset_name}}</t>
-  </si>
-  <si>
-    <t>{{asset_number}}</t>
-  </si>
-  <si>
-    <t>{{currency purchase_price}}</t>
-  </si>
-  <si>
-    <t>{{fmt_date purchase_date}}</t>
-  </si>
-  <si>
-    <t>{{rate}}%</t>
-  </si>
-  <si>
-    <t>{{currency book_val_from}}</t>
-  </si>
-  <si>
-    <t>{{currency accum_dep}}</t>
-  </si>
-  <si>
-    <t>{{currency book_val_to}}</t>
-  </si>
-  <si>
-    <t>{{/each}}</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>{{currency total_book_val_from}}</t>
-  </si>
-  <si>
-    <t>{{currency total_accum_dep}}</t>
-  </si>
-  <si>
-    <t>{{currency total_book_val_to}}</t>
+    <t xml:space="preserve">Accum Dep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book Value {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each groups}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{type_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each lines}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{asset_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{asset_number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency purchase_price}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{fmt_date purchase_date}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{rate}}%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency book_val_from}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency accum_dep}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency book_val_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{/each}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_book_val_from}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_accum_dep}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_book_val_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -104,9 +109,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -147,6 +152,13 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -212,12 +224,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -225,7 +237,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,7 +249,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,23 +334,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.68367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -347,7 +363,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" s="2" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -359,7 +375,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" s="2" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -371,7 +387,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" s="2" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -383,7 +399,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" s="2" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -466,26 +482,37 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="F12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="0" t="s">
+      <c r="G14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="H14" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -495,7 +522,7 @@
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
add tracking to report_dep_schedule
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
@@ -5,103 +5,110 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="447" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
-  <si>
-    <t xml:space="preserve">Depreciation Schedule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{company_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Book Value
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+  <si>
+    <t>Depreciation Schedule</t>
+  </si>
+  <si>
+    <t>{{company_name}}</t>
+  </si>
+  <si>
+    <t>From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Tracking-1</t>
+  </si>
+  <si>
+    <t>Tracking-2</t>
+  </si>
+  <si>
+    <t>Purchase Price</t>
+  </si>
+  <si>
+    <t>Purchase Date</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Book Value
 {{fmt_date date_from}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Accum Dep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Book Value {{fmt_date date_to}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{#each groups}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{type_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{#each lines}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{asset_name}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{asset_number}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency purchase_price}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{fmt_date purchase_date}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{rate}}%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency book_val_from}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency accum_dep}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency book_val_to}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{/each}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_book_val_from}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_accum_dep}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{currency total_book_val_to}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
+    <t>Accum Dep</t>
+  </si>
+  <si>
+    <t>Book Value {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t>{{#each groups}}</t>
+  </si>
+  <si>
+    <t>{{type_name}}</t>
+  </si>
+  <si>
+    <t>{{#each lines}}</t>
+  </si>
+  <si>
+    <t>{{asset_name}}</t>
+  </si>
+  <si>
+    <t>{{asset_number}}</t>
+  </si>
+  <si>
+    <t>{{track_name}}</t>
+  </si>
+  <si>
+    <t>{{track2_name}}</t>
+  </si>
+  <si>
+    <t>{{currency purchase_price}}</t>
+  </si>
+  <si>
+    <t>{{fmt_date purchase_date}}</t>
+  </si>
+  <si>
+    <t>{{rate}}%</t>
+  </si>
+  <si>
+    <t>{{currency book_val_from}}</t>
+  </si>
+  <si>
+    <t>{{currency accum_dep}}</t>
+  </si>
+  <si>
+    <t>{{currency book_val_to}}</t>
+  </si>
+  <si>
+    <t>{{/each}}</t>
+  </si>
+  <si>
+    <t>{{currency total_book_val_from}}</t>
+  </si>
+  <si>
+    <t>{{currency total_accum_dep}}</t>
+  </si>
+  <si>
+    <t>{{currency total_book_val_to}}</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -109,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -334,23 +341,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -362,6 +369,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -374,6 +383,8 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -386,6 +397,8 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -398,6 +411,8 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
@@ -408,6 +423,8 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" s="4" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -425,104 +442,118 @@
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A14:G14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
improve depricate schedule report
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
@@ -5,113 +5,121 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="447" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
-  <si>
-    <t>Depreciation Schedule</t>
-  </si>
-  <si>
-    <t>{{company_name}}</t>
-  </si>
-  <si>
-    <t>From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Tracking-1</t>
-  </si>
-  <si>
-    <t>Tracking-2</t>
-  </si>
-  <si>
-    <t>Purchase Price</t>
-  </si>
-  <si>
-    <t>Purchase Date</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Book Value
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+  <si>
+    <t xml:space="preserve">Depreciation Schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{company_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracking-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracking-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book Value
 {{fmt_date date_from}}</t>
   </si>
   <si>
-    <t>Accum Dep</t>
-  </si>
-  <si>
-    <t>Book Value {{fmt_date date_to}}</t>
-  </si>
-  <si>
-    <t>{{#each groups}}</t>
-  </si>
-  <si>
-    <t>{{type_name}}</t>
-  </si>
-  <si>
-    <t>{{#each lines}}</t>
-  </si>
-  <si>
-    <t>{{asset_name}}</t>
-  </si>
-  <si>
-    <t>{{asset_number}}</t>
-  </si>
-  <si>
-    <t>{{track_name}}</t>
-  </si>
-  <si>
-    <t>{{track2_name}}</t>
-  </si>
-  <si>
-    <t>{{currency purchase_price}}</t>
-  </si>
-  <si>
-    <t>{{fmt_date purchase_date}}</t>
-  </si>
-  <si>
-    <t>{{rate}}%</t>
-  </si>
-  <si>
-    <t>{{currency book_val_from}}</t>
-  </si>
-  <si>
-    <t>{{currency accum_dep}}</t>
-  </si>
-  <si>
-    <t>{{currency book_val_to}}</t>
-  </si>
-  <si>
-    <t>{{/each}}</t>
-  </si>
-  <si>
-    <t>{{currency total_book_val_from}}</t>
-  </si>
-  <si>
-    <t>{{currency total_accum_dep}}</t>
-  </si>
-  <si>
-    <t>{{currency total_book_val_to}}</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>{{currency total_purchase_price}}</t>
+    <t xml:space="preserve">Accum Dep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book Value {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each groups}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{type_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each lines}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{asset_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{asset_number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{track_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{track2_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency purchase_price}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{fmt_date purchase_date}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{rate}}%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency book_val_from}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency accum_dep}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency book_val_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{/each}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total {{type_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_purchase_price}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_book_val_from}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_accum_dep}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency total_book_val_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -119,9 +127,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,6 +152,87 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF800000"/>
       <name val="Arial"/>
@@ -161,20 +250,12 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +264,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -200,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -208,8 +331,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -233,79 +371,143 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFEEEEEE"/>
-      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -321,7 +523,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -350,21 +552,21 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -471,7 +673,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -518,14 +720,20 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="H12" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,24 +743,24 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +774,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
improve report fixed_asset & dep_schedule Y gl_details
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/fixed_asset.xlsx
@@ -255,7 +255,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,7 +301,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -314,12 +314,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000080"/>
         <bgColor rgb="FF000080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -420,7 +414,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -429,7 +423,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,6 +431,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,12 +443,20 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -503,7 +509,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -553,7 +559,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -565,7 +571,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.37"/>
   </cols>
   <sheetData>
@@ -581,7 +587,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -595,7 +601,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="4" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -609,7 +615,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" s="4" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -623,7 +629,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="4" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -635,35 +641,35 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" s="4" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" s="7" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -673,7 +679,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -720,19 +726,19 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -742,35 +748,33 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="6" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="8" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>